<commit_message>
Init state to check available tickets
Changes made in initialization (Init) states to validate pending tickets prior to initialize Immi website
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck_1.0/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck_1.0/IAA_VevoCheck/Data/Config.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
+    <sheet name="Messages" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="180">
   <si>
     <t>Name</t>
   </si>
@@ -176,27 +177,6 @@
     <t>OracleCRM_URL_PROD</t>
   </si>
   <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>OperatingEnvironment</t>
-  </si>
-  <si>
-    <t>Current operating environment. Options are DEV, TEST, STAGING and PROD (Type: Text)</t>
-  </si>
-  <si>
-    <t>EmailOnSuccessFlag</t>
-  </si>
-  <si>
-    <t>EmailOnSuccess</t>
-  </si>
-  <si>
-    <t>Set this to True to send emails on successful completion (Type: Boolean)</t>
-  </si>
-  <si>
-    <t>SSO_RPA00001</t>
-  </si>
-  <si>
     <t>SSO_rpa00001</t>
   </si>
   <si>
@@ -324,13 +304,271 @@
   </si>
   <si>
     <t>RPA could not complete this Vevo check. Incorrect data provided - Country of Document field label incorrect or missing - should be "Country of Document:"</t>
+  </si>
+  <si>
+    <t>VevoFileNamePrefix</t>
+  </si>
+  <si>
+    <t>VevoFileNamePattern</t>
+  </si>
+  <si>
+    <t>VEVO Visa Details Check*</t>
+  </si>
+  <si>
+    <t>VEVO Visa Details Check_</t>
+  </si>
+  <si>
+    <t>DownloadLocation</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Downloads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefix for Immi website sreach result in case no pdf found </t>
+  </si>
+  <si>
+    <t>File name pattern for all document retrived from Immi website</t>
+  </si>
+  <si>
+    <t>File path for all document retrived from Immi website</t>
+  </si>
+  <si>
+    <t>Row {0} updated, {1}</t>
+  </si>
+  <si>
+    <t>LogMessage_UpdatedProforma</t>
+  </si>
+  <si>
+    <t>Row {0} skipped, {1}</t>
+  </si>
+  <si>
+    <t>LogMessage_SkippedProforma</t>
+  </si>
+  <si>
+    <t>System Error</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>UniFi Unknown Error</t>
+  </si>
+  <si>
+    <t>9.1-12.9</t>
+  </si>
+  <si>
+    <t>SystemError_UnhandledUniFi</t>
+  </si>
+  <si>
+    <t>I couldn't save the email to {0}</t>
+  </si>
+  <si>
+    <t>Network Error</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>SystemError_SaveEmail</t>
+  </si>
+  <si>
+    <t>I couldn't update row {0} due to: {1}</t>
+  </si>
+  <si>
+    <t>UniFi Updating Error</t>
+  </si>
+  <si>
+    <t>12.1-9</t>
+  </si>
+  <si>
+    <t>SystemError_ProformaEntry</t>
+  </si>
+  <si>
+    <t>I got lost while navigating to {0}</t>
+  </si>
+  <si>
+    <t>UniFi Navigation Error</t>
+  </si>
+  <si>
+    <t>9.7-10</t>
+  </si>
+  <si>
+    <t>SystemError_NavigateUniFi</t>
+  </si>
+  <si>
+    <t>Login issue as {0} to UniFi at {1}: {2} at {3}</t>
+  </si>
+  <si>
+    <t>UniFi Login Error</t>
+  </si>
+  <si>
+    <t>9.1-5</t>
+  </si>
+  <si>
+    <t>SystemError_LoginUniFi</t>
+  </si>
+  <si>
+    <t>I couldn't scrape proforma data from the email {0}</t>
+  </si>
+  <si>
+    <t>Unknown Scrape Error</t>
+  </si>
+  <si>
+    <t>7.1-6</t>
+  </si>
+  <si>
+    <t>SystemError_UnhandledExchange</t>
+  </si>
+  <si>
+    <t>Problems checking {0} as {1}: {2} at {3}</t>
+  </si>
+  <si>
+    <t>Exchange Error</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>SystemError_CheckExchange</t>
+  </si>
+  <si>
+    <t>Problems with {0}'s mail: {1} at: {2}</t>
+  </si>
+  <si>
+    <t>SystemError_InitExchange</t>
+  </si>
+  <si>
+    <t>I couldn't create the folder at {0}</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>SystemError_CreateFolder</t>
+  </si>
+  <si>
+    <t>Problems loading {0} for Acc lookup: {1} at: {2}</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>SystemError_AccountantFile</t>
+  </si>
+  <si>
+    <t>The RM number is missing or the email is not a proforma template</t>
+  </si>
+  <si>
+    <t>Invalid RM Number</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>RuleException_ValidateRMNum</t>
+  </si>
+  <si>
+    <t>I wasn't able to update {0} as the rows were: {1}</t>
+  </si>
+  <si>
+    <t>No Updated Entries</t>
+  </si>
+  <si>
+    <t>10.2-11.3</t>
+  </si>
+  <si>
+    <t>RuleException_UpdateProforma</t>
+  </si>
+  <si>
+    <t>I couldn't validate {0} in the proforma email</t>
+  </si>
+  <si>
+    <t>Invalid Proforma Data</t>
+  </si>
+  <si>
+    <t>7.2-6</t>
+  </si>
+  <si>
+    <t>RuleException_ValidateProforma</t>
+  </si>
+  <si>
+    <t>I searched for {0} and found no results</t>
+  </si>
+  <si>
+    <t>No Search Results</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>RuleException_SearchRMNum</t>
+  </si>
+  <si>
+    <t>I couldn't match {0} to an accountant name</t>
+  </si>
+  <si>
+    <t>Accountant Not Found</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>RuleException_SearchAccountant</t>
+  </si>
+  <si>
+    <t>I couldn't find any emails in {0}</t>
+  </si>
+  <si>
+    <t>No Emails Found</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>I couldn't get my settings from the config: {0}</t>
+  </si>
+  <si>
+    <t>Config Not Initialised</t>
+  </si>
+  <si>
+    <t>I couldn't find my operation mode asset at OperatingEnvironment</t>
+  </si>
+  <si>
+    <t>Mode Asset Missing</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Extras</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>RuleException_NoTicketsToProcess</t>
+  </si>
+  <si>
+    <t>OracleCRM_URL_</t>
+  </si>
+  <si>
+    <t>OracleCRM_URL</t>
+  </si>
+  <si>
+    <t>Credentials_ImmiAccount</t>
+  </si>
+  <si>
+    <t>Credentials_CRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -362,6 +600,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -384,17 +628,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -678,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -728,8 +976,8 @@
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>82</v>
+      <c r="B2" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -740,8 +988,8 @@
       <c r="A4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>81</v>
+      <c r="B4" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -749,104 +997,104 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>67</v>
+      <c r="B6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>68</v>
+      <c r="B7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>69</v>
+      <c r="B8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>70</v>
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>71</v>
+      <c r="A11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
         <v>72</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1846,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2077,91 +2325,128 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3121,10 +3406,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3170,48 +3455,28 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4205,10 +4470,366 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="83.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to Get Transaction state
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck_1.0/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck_1.0/IAA_VevoCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="186">
   <si>
     <t>Name</t>
   </si>
@@ -66,9 +66,6 @@
     <t>ExScreenshotsFolderPath</t>
   </si>
   <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
     <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
   </si>
   <si>
@@ -562,6 +559,27 @@
   </si>
   <si>
     <t>Credentials_CRM</t>
+  </si>
+  <si>
+    <t>International RPA Vevo Check</t>
+  </si>
+  <si>
+    <t>OracleCRM_TabHeader</t>
+  </si>
+  <si>
+    <t>Vevo Check Out</t>
+  </si>
+  <si>
+    <t>OracleCRM_VevoCheckOut</t>
+  </si>
+  <si>
+    <t>Deafult dashboard tab header name</t>
+  </si>
+  <si>
+    <t>IAS Category name for Vevo Check Out queue</t>
+  </si>
+  <si>
+    <t>C:\Users\uqmgupt1\Downloads</t>
   </si>
 </sst>
 </file>
@@ -927,7 +945,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -974,127 +992,127 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
         <v>45</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
         <v>65</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
         <v>67</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
         <v>69</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
         <v>71</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2085,6 +2103,7 @@
     <hyperlink ref="B11" r:id="rId3"/>
     <hyperlink ref="B13" r:id="rId4"/>
     <hyperlink ref="B14" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2094,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2192,256 +2211,276 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>1000</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>15000</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>60000</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>0.6</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>0.8</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>0.9</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>32</v>
-      </c>
-      <c r="C20" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
         <v>40</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
         <v>95</v>
       </c>
-      <c r="B36" t="s">
-        <v>96</v>
-      </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" t="s">
         <v>98</v>
       </c>
-      <c r="B38" t="s">
-        <v>99</v>
-      </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" t="s">
+        <v>179</v>
+      </c>
+      <c r="C42" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>182</v>
+      </c>
+      <c r="B43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" t="s">
+        <v>184</v>
+      </c>
+    </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3401,6 +3440,7 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3408,8 +3448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3455,24 +3495,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4481,7 +4521,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4498,13 +4538,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>3</v>
@@ -4512,25 +4552,25 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E3" s="11"/>
     </row>
@@ -4540,292 +4580,292 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D23" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
         <v>28</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>29</v>
-      </c>
-      <c r="D27" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
         <v>34</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>35</v>
-      </c>
-      <c r="D28" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRM Unit test and changes to get transaction details
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck_1.0/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck_1.0/IAA_VevoCheck/Data/Config.xlsx
@@ -945,7 +945,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2113,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes to Init and Process transaction
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck_1.0/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck_1.0/IAA_VevoCheck/Data/Config.xlsx
@@ -249,30 +249,6 @@
     <t>IAA_VevoCheck-1.0</t>
   </si>
   <si>
-    <t>ErrorMessage_label_Missing_FamilyName</t>
-  </si>
-  <si>
-    <t>ErrorMessage_value_Missing_FamilyName</t>
-  </si>
-  <si>
-    <t>ErrorMessage_label_Missing_DateOfBirth</t>
-  </si>
-  <si>
-    <t>ErrorMessage_value_Missing_DateOfBirth</t>
-  </si>
-  <si>
-    <t>ErrorMessage_label_Missing_PassportNumber</t>
-  </si>
-  <si>
-    <t>ErrorMessage_value_Missing_PassportNumber</t>
-  </si>
-  <si>
-    <t>ErrorMessage_label_Missing_CountryOfDocument</t>
-  </si>
-  <si>
-    <t>ErrorMessage_value_Missing_CountryOfDocument</t>
-  </si>
-  <si>
     <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name field label incorrect or missing - should be "Family Name:"</t>
   </si>
   <si>
@@ -282,9 +258,6 @@
     <t>RPA could not complete this Vevo check. Incorrect data provided - Family Name value is missing.</t>
   </si>
   <si>
-    <t>ErrorMessage_IncorrectFormat_DateOfBirth</t>
-  </si>
-  <si>
     <t>RPA could not complete this Vevo check. Incorrect data provided - Date of Birth field label incorrect or missing - should be "Date of Birth:".</t>
   </si>
   <si>
@@ -580,6 +553,33 @@
   </si>
   <si>
     <t>C:\Users\uqmgupt1\Downloads</t>
+  </si>
+  <si>
+    <t>ErrMsg_value_Missing_FamilyName</t>
+  </si>
+  <si>
+    <t>ErrMsg_label_Missing_FamilyName</t>
+  </si>
+  <si>
+    <t>ErrMsg_label_Missing_DateOfBirth</t>
+  </si>
+  <si>
+    <t>ErrMsg_value_Missing_DateOfBirth</t>
+  </si>
+  <si>
+    <t>ErrMsg_IncorrectFormat_DateOfBirth</t>
+  </si>
+  <si>
+    <t>ErrMsg_label_Missing_PassportNumber</t>
+  </si>
+  <si>
+    <t>ErrMsg_value_Missing_PassportNumber</t>
+  </si>
+  <si>
+    <t>ErrMsg_label_Missing_CountryOfDocument</t>
+  </si>
+  <si>
+    <t>ErrMsg_value_Missing_CountryOfDocument</t>
   </si>
 </sst>
 </file>
@@ -2114,7 +2114,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2211,7 +2211,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -2344,141 +2344,141 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" t="s">
         <v>75</v>
-      </c>
-      <c r="B25" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>181</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" t="s">
         <v>80</v>
-      </c>
-      <c r="B31" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>184</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" t="s">
         <v>82</v>
-      </c>
-      <c r="B33" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B40" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B42" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C42" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C43" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3495,7 +3495,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
@@ -3506,7 +3506,7 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>51</v>
@@ -4538,13 +4538,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>3</v>
@@ -4552,25 +4552,25 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="7" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E3" s="11"/>
     </row>
@@ -4580,223 +4580,223 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D23" s="9"/>
     </row>
@@ -4805,10 +4805,10 @@
         <v>30</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
         <v>32</v>
@@ -4819,10 +4819,10 @@
         <v>39</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
         <v>41</v>
@@ -4852,20 +4852,20 @@
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Get Transactions and Init state
</commit_message>
<xml_diff>
--- a/Processes/IAA_VevoCheck_1.0/IAA_VevoCheck/Data/Config.xlsx
+++ b/Processes/IAA_VevoCheck_1.0/IAA_VevoCheck/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="149">
   <si>
     <t>Name</t>
   </si>
@@ -457,6 +457,18 @@
   </si>
   <si>
     <t>SystemException_CRM</t>
+  </si>
+  <si>
+    <t>ImmiErrorVevoInput</t>
+  </si>
+  <si>
+    <t>An exception occurred while entering Vevo details on Immi website</t>
+  </si>
+  <si>
+    <t>ImmiErrorDownloadSearchResult</t>
+  </si>
+  <si>
+    <t>An exception occurred while retriving Vevo serach result from Immi website</t>
   </si>
 </sst>
 </file>
@@ -523,7 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -531,13 +543,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1988,10 +1996,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:C25"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2163,202 +2171,202 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>39</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>40</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" t="s">
-        <v>75</v>
-      </c>
-    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>115</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" t="s">
-        <v>90</v>
-      </c>
-    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>85</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>86</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>88</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>89</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>98</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" t="s">
-        <v>105</v>
-      </c>
-    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>104</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>103</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3315,6 +3323,7 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4395,240 +4404,230 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="83.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="83.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>108</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="8"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="8"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="8"/>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
-      <c r="C30" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>